<commit_message>
Agendas for meetings 24 and 25
</commit_message>
<xml_diff>
--- a/Documents/Management/Weekly Reports Tracking.xlsx
+++ b/Documents/Management/Weekly Reports Tracking.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Documents\MEng- York\Yr-3 (2013-2014)\Sweng\GitHub\SWENG\Documents\Management\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="21020" yWindow="0" windowWidth="17380" windowHeight="21100" tabRatio="500"/>
+    <workbookView xWindow="21015" yWindow="0" windowWidth="17385" windowHeight="21105" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="32">
   <si>
     <t>Weekly Reports Checklist</t>
   </si>
@@ -121,7 +126,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -137,11 +142,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -201,34 +201,33 @@
   </borders>
   <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -264,6 +263,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -592,13 +599,13 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="10" max="10" width="12.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.375" customWidth="1"/>
+    <col min="10" max="10" width="12.125" customWidth="1"/>
     <col min="11" max="11" width="12" customWidth="1"/>
     <col min="12" max="12" width="18" customWidth="1"/>
   </cols>
@@ -652,34 +659,34 @@
       <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="C5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>21</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="8" t="s">
+      <c r="G5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="7" t="s">
         <v>28</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="4" t="s">
         <v>21</v>
       </c>
     </row>
@@ -687,29 +694,29 @@
       <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="6" t="s">
+      <c r="C6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8" t="s">
+      <c r="G6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7" t="s">
         <v>27</v>
       </c>
       <c r="L6" s="2" t="s">
@@ -720,27 +727,27 @@
       <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" s="5" t="s">
+      <c r="C7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
       <c r="L7" s="2" t="s">
         <v>29</v>
       </c>
@@ -749,29 +756,29 @@
       <c r="B8" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="7" t="s">
+      <c r="C8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
+      <c r="G8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
       <c r="L8" s="2" t="s">
         <v>31</v>
       </c>
@@ -780,27 +787,27 @@
       <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" s="5" t="s">
+      <c r="C9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>21</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
       <c r="L9" s="2" t="s">
         <v>29</v>
       </c>
@@ -809,26 +816,26 @@
       <c r="B10" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="6" t="s">
+      <c r="C10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -836,45 +843,49 @@
       <c r="B11" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I11" s="4"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="6"/>
+      <c r="C11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="5"/>
     </row>
     <row r="12" spans="1:12">
       <c r="B12" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
     </row>
   </sheetData>
   <sortState ref="C4:L4">

</xml_diff>